<commit_message>
Added a good number of equip. to database
Also added some temp techs to Austria to avoid so many errors
</commit_message>
<xml_diff>
--- a/Equipment codes for OOBs.xlsx
+++ b/Equipment codes for OOBs.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="441">
   <si>
     <t>Equipment Code</t>
   </si>
@@ -46,22 +46,7 @@
     <t>Reference Guide for making Order of Battles (ORBAT) by Killerrabbit</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>NB! </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>All codes are case-sensitive. It's an good idea to copy/pase when working with them.</t>
-    </r>
+    <t>NB! All codes are case-sensitive. It's an good idea to copy/pase when working with them.</t>
   </si>
   <si>
     <t>Subtechs don't require the previous Gen model of itself, but needs the same Gen model of what it is an subtech of.</t>
@@ -1324,7 +1309,19 @@
     <t>L_Strike_fighter_equipment_1</t>
   </si>
   <si>
+    <t>L_Strike_fighter1</t>
+  </si>
+  <si>
     <t>L_Strike_fighter_equipment_2</t>
+  </si>
+  <si>
+    <t>L_Strike_fighter2</t>
+  </si>
+  <si>
+    <t>L_Strike_fighter_equipment_3</t>
+  </si>
+  <si>
+    <t>L_Strike_fighter3</t>
   </si>
   <si>
     <t>early_helicopter</t>
@@ -1360,6 +1357,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1381,6 +1379,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1425,7 +1424,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1440,6 +1439,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1463,22 +1466,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G186"/>
+  <dimension ref="A1:G189"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="510" topLeftCell="A1" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="510" topLeftCell="A157" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B180" activeCellId="0" sqref="B180"/>
+      <selection pane="bottomLeft" activeCell="A180" activeCellId="0" sqref="A180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="28.4897959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.0051020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2551020408163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="28.0765306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1516,7 +1519,7 @@
       <c r="D3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="3"/>
@@ -1528,7 +1531,7 @@
       <c r="D5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="4"/>
+      <c r="C6" s="5"/>
       <c r="D6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1538,7 +1541,7 @@
       <c r="B7" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="4" t="n">
+      <c r="C7" s="5" t="n">
         <v>1965</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -1552,7 +1555,7 @@
       <c r="B8" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="4" t="n">
+      <c r="C8" s="5" t="n">
         <v>1975</v>
       </c>
       <c r="D8" s="3"/>
@@ -1564,7 +1567,7 @@
       <c r="B9" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="4" t="n">
+      <c r="C9" s="5" t="n">
         <v>1985</v>
       </c>
       <c r="D9" s="3"/>
@@ -1576,7 +1579,7 @@
       <c r="B10" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="4" t="n">
+      <c r="C10" s="5" t="n">
         <v>1995</v>
       </c>
       <c r="D10" s="3"/>
@@ -1588,7 +1591,7 @@
       <c r="B11" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="4" t="n">
+      <c r="C11" s="5" t="n">
         <v>2005</v>
       </c>
       <c r="D11" s="3"/>
@@ -1600,13 +1603,13 @@
       <c r="B12" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="4" t="n">
+      <c r="C12" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="D12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="4"/>
+      <c r="C13" s="5"/>
       <c r="D13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1616,7 +1619,7 @@
       <c r="B14" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="4" t="n">
+      <c r="C14" s="5" t="n">
         <v>1965</v>
       </c>
       <c r="D14" s="3" t="s">
@@ -1630,7 +1633,7 @@
       <c r="B15" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="4" t="n">
+      <c r="C15" s="5" t="n">
         <v>1975</v>
       </c>
       <c r="D15" s="3"/>
@@ -1642,7 +1645,7 @@
       <c r="B16" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="4" t="n">
+      <c r="C16" s="5" t="n">
         <v>1985</v>
       </c>
       <c r="D16" s="3"/>
@@ -1654,7 +1657,7 @@
       <c r="B17" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="4" t="n">
+      <c r="C17" s="5" t="n">
         <v>1995</v>
       </c>
       <c r="D17" s="3"/>
@@ -1666,7 +1669,7 @@
       <c r="B18" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="4" t="n">
+      <c r="C18" s="5" t="n">
         <v>2005</v>
       </c>
       <c r="D18" s="3"/>
@@ -1678,13 +1681,13 @@
       <c r="B19" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="4" t="n">
+      <c r="C19" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="D19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="4"/>
+      <c r="C20" s="5"/>
       <c r="D20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1694,13 +1697,13 @@
       <c r="B21" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="4"/>
+      <c r="C21" s="5"/>
       <c r="D21" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="4"/>
+      <c r="C22" s="5"/>
       <c r="D22" s="3"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1710,7 +1713,7 @@
       <c r="B23" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="4" t="n">
+      <c r="C23" s="5" t="n">
         <v>1965</v>
       </c>
       <c r="D23" s="3" t="s">
@@ -1724,7 +1727,7 @@
       <c r="B24" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="4" t="n">
+      <c r="C24" s="5" t="n">
         <v>1975</v>
       </c>
       <c r="D24" s="3"/>
@@ -1736,13 +1739,13 @@
       <c r="B25" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="C25" s="4" t="n">
+      <c r="C25" s="5" t="n">
         <v>1985</v>
       </c>
       <c r="D25" s="3"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="4"/>
+      <c r="C26" s="5"/>
       <c r="D26" s="3"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1752,7 +1755,7 @@
       <c r="B27" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="4" t="n">
+      <c r="C27" s="5" t="n">
         <v>1975</v>
       </c>
       <c r="D27" s="3" t="s">
@@ -1769,7 +1772,7 @@
       <c r="B28" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="4" t="n">
+      <c r="C28" s="5" t="n">
         <v>1985</v>
       </c>
       <c r="D28" s="3"/>
@@ -1784,7 +1787,7 @@
       <c r="B29" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C29" s="4" t="n">
+      <c r="C29" s="5" t="n">
         <v>1995</v>
       </c>
       <c r="D29" s="3"/>
@@ -1799,7 +1802,7 @@
       <c r="B30" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="C30" s="4" t="n">
+      <c r="C30" s="5" t="n">
         <v>2005</v>
       </c>
       <c r="D30" s="3"/>
@@ -1814,7 +1817,7 @@
       <c r="B31" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="4" t="n">
+      <c r="C31" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="D31" s="3"/>
@@ -1823,7 +1826,7 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C32" s="4"/>
+      <c r="C32" s="5"/>
       <c r="D32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1833,7 +1836,7 @@
       <c r="B33" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="4" t="n">
+      <c r="C33" s="5" t="n">
         <v>1985</v>
       </c>
       <c r="D33" s="3" t="s">
@@ -1847,7 +1850,7 @@
       <c r="B34" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C34" s="4" t="n">
+      <c r="C34" s="5" t="n">
         <v>1995</v>
       </c>
       <c r="D34" s="3"/>
@@ -1859,7 +1862,7 @@
       <c r="B35" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="C35" s="4" t="n">
+      <c r="C35" s="5" t="n">
         <v>2005</v>
       </c>
       <c r="D35" s="3"/>
@@ -1871,13 +1874,13 @@
       <c r="B36" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="C36" s="4" t="n">
+      <c r="C36" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="D36" s="3"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="4"/>
+      <c r="C37" s="5"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
@@ -1886,7 +1889,7 @@
       <c r="B38" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="C38" s="4" t="n">
+      <c r="C38" s="5" t="n">
         <v>1965</v>
       </c>
       <c r="D38" s="3" t="s">
@@ -1906,7 +1909,7 @@
       <c r="B39" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="C39" s="4" t="n">
+      <c r="C39" s="5" t="n">
         <v>1985</v>
       </c>
       <c r="E39" s="0" t="s">
@@ -1926,7 +1929,7 @@
       <c r="B40" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="C40" s="4" t="n">
+      <c r="C40" s="5" t="n">
         <v>2005</v>
       </c>
       <c r="E40" s="0" t="s">
@@ -1940,7 +1943,7 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C41" s="4"/>
+      <c r="C41" s="5"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
@@ -1949,7 +1952,7 @@
       <c r="B42" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="C42" s="4" t="n">
+      <c r="C42" s="5" t="n">
         <v>1965</v>
       </c>
       <c r="D42" s="0" t="s">
@@ -1966,7 +1969,7 @@
       <c r="B43" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="C43" s="4" t="n">
+      <c r="C43" s="5" t="n">
         <v>1985</v>
       </c>
       <c r="D43" s="0" t="s">
@@ -1989,7 +1992,7 @@
       <c r="B44" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="C44" s="4" t="n">
+      <c r="C44" s="5" t="n">
         <v>2005</v>
       </c>
       <c r="D44" s="0" t="s">
@@ -2003,7 +2006,7 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C45" s="4"/>
+      <c r="C45" s="5"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
@@ -2012,7 +2015,7 @@
       <c r="B46" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="C46" s="4" t="n">
+      <c r="C46" s="5" t="n">
         <v>1975</v>
       </c>
       <c r="D46" s="0" t="s">
@@ -2026,7 +2029,7 @@
       <c r="B47" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="C47" s="4" t="n">
+      <c r="C47" s="5" t="n">
         <v>1995</v>
       </c>
       <c r="D47" s="0" t="s">
@@ -2034,7 +2037,7 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C48" s="4"/>
+      <c r="C48" s="5"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
@@ -2043,7 +2046,7 @@
       <c r="B49" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="C49" s="4" t="n">
+      <c r="C49" s="5" t="n">
         <v>1965</v>
       </c>
       <c r="D49" s="0" t="s">
@@ -2063,7 +2066,7 @@
       <c r="B50" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="C50" s="4" t="n">
+      <c r="C50" s="5" t="n">
         <v>1985</v>
       </c>
       <c r="E50" s="0" t="s">
@@ -2080,7 +2083,7 @@
       <c r="B51" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="C51" s="4" t="n">
+      <c r="C51" s="5" t="n">
         <v>2005</v>
       </c>
       <c r="E51" s="0" t="s">
@@ -2094,7 +2097,7 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C52" s="4"/>
+      <c r="C52" s="5"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
@@ -2103,7 +2106,7 @@
       <c r="B53" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="C53" s="4" t="n">
+      <c r="C53" s="5" t="n">
         <v>1965</v>
       </c>
       <c r="D53" s="0" t="s">
@@ -2123,7 +2126,7 @@
       <c r="B54" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="C54" s="4" t="n">
+      <c r="C54" s="5" t="n">
         <v>1985</v>
       </c>
       <c r="E54" s="0" t="s">
@@ -2140,7 +2143,7 @@
       <c r="B55" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="C55" s="4" t="n">
+      <c r="C55" s="5" t="n">
         <v>2005</v>
       </c>
       <c r="E55" s="0" t="s">
@@ -2154,7 +2157,7 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C56" s="4"/>
+      <c r="C56" s="5"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
@@ -2163,7 +2166,7 @@
       <c r="B57" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="C57" s="4" t="n">
+      <c r="C57" s="5" t="n">
         <v>1965</v>
       </c>
       <c r="D57" s="0" t="s">
@@ -2180,7 +2183,7 @@
       <c r="B58" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="C58" s="4" t="n">
+      <c r="C58" s="5" t="n">
         <v>1985</v>
       </c>
       <c r="D58" s="0" t="s">
@@ -2200,7 +2203,7 @@
       <c r="B59" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="C59" s="4" t="n">
+      <c r="C59" s="5" t="n">
         <v>2005</v>
       </c>
       <c r="D59" s="0" t="s">
@@ -2214,7 +2217,7 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C60" s="4"/>
+      <c r="C60" s="5"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
@@ -2223,7 +2226,7 @@
       <c r="B61" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="C61" s="4" t="n">
+      <c r="C61" s="5" t="n">
         <v>1975</v>
       </c>
       <c r="D61" s="0" t="s">
@@ -2237,7 +2240,7 @@
       <c r="B62" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="C62" s="4" t="n">
+      <c r="C62" s="5" t="n">
         <v>1995</v>
       </c>
       <c r="D62" s="0" t="s">
@@ -2245,7 +2248,7 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C63" s="4"/>
+      <c r="C63" s="5"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
@@ -2254,7 +2257,7 @@
       <c r="B64" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="C64" s="4" t="n">
+      <c r="C64" s="5" t="n">
         <v>1965</v>
       </c>
       <c r="D64" s="0" t="s">
@@ -2277,7 +2280,7 @@
       <c r="B65" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="C65" s="4" t="n">
+      <c r="C65" s="5" t="n">
         <v>1985</v>
       </c>
       <c r="E65" s="0" t="s">
@@ -2297,7 +2300,7 @@
       <c r="B66" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="C66" s="4" t="n">
+      <c r="C66" s="5" t="n">
         <v>2005</v>
       </c>
       <c r="E66" s="0" t="s">
@@ -2311,7 +2314,7 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C67" s="4"/>
+      <c r="C67" s="5"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
@@ -2320,7 +2323,7 @@
       <c r="B68" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="C68" s="4" t="n">
+      <c r="C68" s="5" t="n">
         <v>1965</v>
       </c>
       <c r="D68" s="0" t="s">
@@ -2334,7 +2337,7 @@
       <c r="B69" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="C69" s="4" t="n">
+      <c r="C69" s="5" t="n">
         <v>1985</v>
       </c>
       <c r="D69" s="0" t="s">
@@ -2354,7 +2357,7 @@
       <c r="B70" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="C70" s="4" t="n">
+      <c r="C70" s="5" t="n">
         <v>2005</v>
       </c>
       <c r="D70" s="0" t="s">
@@ -2365,7 +2368,7 @@
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C71" s="4"/>
+      <c r="C71" s="5"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
@@ -2374,7 +2377,7 @@
       <c r="B72" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="C72" s="4" t="n">
+      <c r="C72" s="5" t="n">
         <v>1975</v>
       </c>
       <c r="D72" s="0" t="s">
@@ -2388,7 +2391,7 @@
       <c r="B73" s="0" t="s">
         <v>168</v>
       </c>
-      <c r="C73" s="4" t="n">
+      <c r="C73" s="5" t="n">
         <v>1995</v>
       </c>
       <c r="D73" s="0" t="s">
@@ -2396,7 +2399,7 @@
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C74" s="4"/>
+      <c r="C74" s="5"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
@@ -2405,13 +2408,13 @@
       <c r="B75" s="0" t="s">
         <v>170</v>
       </c>
-      <c r="C75" s="4"/>
+      <c r="C75" s="5"/>
       <c r="D75" s="3" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C76" s="4"/>
+      <c r="C76" s="5"/>
       <c r="D76" s="3"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2421,7 +2424,7 @@
       <c r="B77" s="0" t="s">
         <v>173</v>
       </c>
-      <c r="C77" s="4" t="n">
+      <c r="C77" s="5" t="n">
         <v>1965</v>
       </c>
       <c r="D77" s="3" t="s">
@@ -2435,7 +2438,7 @@
       <c r="B78" s="0" t="s">
         <v>176</v>
       </c>
-      <c r="C78" s="4" t="n">
+      <c r="C78" s="5" t="n">
         <v>1975</v>
       </c>
       <c r="D78" s="3"/>
@@ -2447,7 +2450,7 @@
       <c r="B79" s="0" t="s">
         <v>178</v>
       </c>
-      <c r="C79" s="4" t="n">
+      <c r="C79" s="5" t="n">
         <v>1985</v>
       </c>
       <c r="D79" s="3"/>
@@ -2459,7 +2462,7 @@
       <c r="B80" s="0" t="s">
         <v>180</v>
       </c>
-      <c r="C80" s="4" t="n">
+      <c r="C80" s="5" t="n">
         <v>1995</v>
       </c>
       <c r="D80" s="3"/>
@@ -2471,7 +2474,7 @@
       <c r="B81" s="0" t="s">
         <v>182</v>
       </c>
-      <c r="C81" s="4" t="n">
+      <c r="C81" s="5" t="n">
         <v>2005</v>
       </c>
       <c r="D81" s="3"/>
@@ -2483,13 +2486,13 @@
       <c r="B82" s="0" t="s">
         <v>184</v>
       </c>
-      <c r="C82" s="4" t="n">
+      <c r="C82" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="D82" s="3"/>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C83" s="4"/>
+      <c r="C83" s="5"/>
       <c r="D83" s="3"/>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2499,7 +2502,7 @@
       <c r="B84" s="0" t="s">
         <v>186</v>
       </c>
-      <c r="C84" s="4" t="n">
+      <c r="C84" s="5" t="n">
         <v>1965</v>
       </c>
       <c r="D84" s="3" t="s">
@@ -2513,7 +2516,7 @@
       <c r="B85" s="0" t="s">
         <v>186</v>
       </c>
-      <c r="C85" s="4" t="n">
+      <c r="C85" s="5" t="n">
         <v>1975</v>
       </c>
       <c r="D85" s="0" t="s">
@@ -2527,7 +2530,7 @@
       <c r="B86" s="0" t="s">
         <v>186</v>
       </c>
-      <c r="C86" s="4" t="n">
+      <c r="C86" s="5" t="n">
         <v>1985</v>
       </c>
       <c r="D86" s="0" t="s">
@@ -2544,7 +2547,7 @@
       <c r="B87" s="0" t="s">
         <v>186</v>
       </c>
-      <c r="C87" s="4" t="n">
+      <c r="C87" s="5" t="n">
         <v>1995</v>
       </c>
       <c r="D87" s="0" t="s">
@@ -2558,7 +2561,7 @@
       <c r="B88" s="0" t="s">
         <v>186</v>
       </c>
-      <c r="C88" s="4" t="n">
+      <c r="C88" s="5" t="n">
         <v>2005</v>
       </c>
       <c r="D88" s="0" t="s">
@@ -2575,7 +2578,7 @@
       <c r="B89" s="0" t="s">
         <v>186</v>
       </c>
-      <c r="C89" s="4" t="n">
+      <c r="C89" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="D89" s="0" t="s">
@@ -2592,7 +2595,7 @@
       <c r="B91" s="0" t="s">
         <v>196</v>
       </c>
-      <c r="C91" s="4" t="n">
+      <c r="C91" s="5" t="n">
         <v>1965</v>
       </c>
       <c r="D91" s="3" t="s">
@@ -2606,7 +2609,7 @@
       <c r="B92" s="0" t="s">
         <v>199</v>
       </c>
-      <c r="C92" s="4" t="n">
+      <c r="C92" s="5" t="n">
         <v>1975</v>
       </c>
       <c r="D92" s="0" t="s">
@@ -2620,7 +2623,7 @@
       <c r="B93" s="0" t="s">
         <v>201</v>
       </c>
-      <c r="C93" s="4" t="n">
+      <c r="C93" s="5" t="n">
         <v>1985</v>
       </c>
       <c r="D93" s="0" t="s">
@@ -2634,7 +2637,7 @@
       <c r="B94" s="0" t="s">
         <v>203</v>
       </c>
-      <c r="C94" s="4" t="n">
+      <c r="C94" s="5" t="n">
         <v>1995</v>
       </c>
       <c r="D94" s="0" t="s">
@@ -2648,7 +2651,7 @@
       <c r="B95" s="0" t="s">
         <v>205</v>
       </c>
-      <c r="C95" s="4" t="n">
+      <c r="C95" s="5" t="n">
         <v>2005</v>
       </c>
       <c r="D95" s="0" t="s">
@@ -2662,7 +2665,7 @@
       <c r="B96" s="0" t="s">
         <v>207</v>
       </c>
-      <c r="C96" s="4" t="n">
+      <c r="C96" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="D96" s="0" t="s">
@@ -2670,7 +2673,7 @@
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C97" s="4"/>
+      <c r="C97" s="5"/>
       <c r="D97" s="3"/>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2680,7 +2683,7 @@
       <c r="B98" s="0" t="s">
         <v>209</v>
       </c>
-      <c r="C98" s="4" t="n">
+      <c r="C98" s="5" t="n">
         <v>1965</v>
       </c>
       <c r="D98" s="3" t="s">
@@ -2697,7 +2700,7 @@
       <c r="B99" s="0" t="s">
         <v>209</v>
       </c>
-      <c r="C99" s="4" t="n">
+      <c r="C99" s="5" t="n">
         <v>1975</v>
       </c>
       <c r="D99" s="3"/>
@@ -2712,7 +2715,7 @@
       <c r="B100" s="0" t="s">
         <v>209</v>
       </c>
-      <c r="C100" s="4" t="n">
+      <c r="C100" s="5" t="n">
         <v>1985</v>
       </c>
       <c r="D100" s="3"/>
@@ -2733,7 +2736,7 @@
       <c r="B101" s="0" t="s">
         <v>209</v>
       </c>
-      <c r="C101" s="4" t="n">
+      <c r="C101" s="5" t="n">
         <v>1995</v>
       </c>
       <c r="D101" s="3"/>
@@ -2754,7 +2757,7 @@
       <c r="B102" s="0" t="s">
         <v>209</v>
       </c>
-      <c r="C102" s="4" t="n">
+      <c r="C102" s="5" t="n">
         <v>2005</v>
       </c>
       <c r="D102" s="3"/>
@@ -2769,7 +2772,7 @@
       <c r="B103" s="0" t="s">
         <v>209</v>
       </c>
-      <c r="C103" s="4" t="n">
+      <c r="C103" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="D103" s="3"/>
@@ -2784,7 +2787,7 @@
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C104" s="4"/>
+      <c r="C104" s="5"/>
       <c r="D104" s="3"/>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2794,7 +2797,7 @@
       <c r="B105" s="0" t="s">
         <v>229</v>
       </c>
-      <c r="C105" s="4" t="n">
+      <c r="C105" s="5" t="n">
         <v>1965</v>
       </c>
       <c r="D105" s="3" t="s">
@@ -2811,7 +2814,7 @@
       <c r="B106" s="0" t="s">
         <v>233</v>
       </c>
-      <c r="C106" s="4" t="n">
+      <c r="C106" s="5" t="n">
         <v>1975</v>
       </c>
       <c r="D106" s="0" t="s">
@@ -2825,7 +2828,7 @@
       <c r="B107" s="0" t="s">
         <v>235</v>
       </c>
-      <c r="C107" s="4" t="n">
+      <c r="C107" s="5" t="n">
         <v>1985</v>
       </c>
       <c r="D107" s="0" t="s">
@@ -2842,7 +2845,7 @@
       <c r="B108" s="0" t="s">
         <v>238</v>
       </c>
-      <c r="C108" s="4" t="n">
+      <c r="C108" s="5" t="n">
         <v>1995</v>
       </c>
       <c r="D108" s="0" t="s">
@@ -2859,7 +2862,7 @@
       <c r="B109" s="0" t="s">
         <v>241</v>
       </c>
-      <c r="C109" s="4" t="n">
+      <c r="C109" s="5" t="n">
         <v>2005</v>
       </c>
       <c r="D109" s="0" t="s">
@@ -2876,7 +2879,7 @@
       <c r="B110" s="0" t="s">
         <v>244</v>
       </c>
-      <c r="C110" s="4" t="n">
+      <c r="C110" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="D110" s="0" t="s">
@@ -2884,7 +2887,7 @@
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C111" s="4"/>
+      <c r="C111" s="5"/>
       <c r="D111" s="3"/>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2894,7 +2897,7 @@
       <c r="B112" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="C112" s="4" t="n">
+      <c r="C112" s="5" t="n">
         <v>1965</v>
       </c>
       <c r="D112" s="3" t="s">
@@ -2908,7 +2911,7 @@
       <c r="B113" s="0" t="s">
         <v>249</v>
       </c>
-      <c r="C113" s="4" t="n">
+      <c r="C113" s="5" t="n">
         <v>1975</v>
       </c>
       <c r="D113" s="0" t="s">
@@ -2922,7 +2925,7 @@
       <c r="B114" s="0" t="s">
         <v>251</v>
       </c>
-      <c r="C114" s="4" t="n">
+      <c r="C114" s="5" t="n">
         <v>1985</v>
       </c>
       <c r="D114" s="0" t="s">
@@ -2936,7 +2939,7 @@
       <c r="B115" s="0" t="s">
         <v>253</v>
       </c>
-      <c r="C115" s="4" t="n">
+      <c r="C115" s="5" t="n">
         <v>1995</v>
       </c>
       <c r="D115" s="0" t="s">
@@ -2950,7 +2953,7 @@
       <c r="B116" s="0" t="s">
         <v>255</v>
       </c>
-      <c r="C116" s="4" t="n">
+      <c r="C116" s="5" t="n">
         <v>2005</v>
       </c>
       <c r="D116" s="0" t="s">
@@ -2964,7 +2967,7 @@
       <c r="B117" s="0" t="s">
         <v>257</v>
       </c>
-      <c r="C117" s="4" t="n">
+      <c r="C117" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="D117" s="0" t="s">
@@ -2981,7 +2984,7 @@
       <c r="B119" s="0" t="s">
         <v>258</v>
       </c>
-      <c r="C119" s="4" t="n">
+      <c r="C119" s="5" t="n">
         <v>1965</v>
       </c>
       <c r="D119" s="3" t="s">
@@ -3001,7 +3004,7 @@
       <c r="B120" s="0" t="s">
         <v>262</v>
       </c>
-      <c r="C120" s="4" t="n">
+      <c r="C120" s="5" t="n">
         <v>1975</v>
       </c>
       <c r="D120" s="3"/>
@@ -3019,7 +3022,7 @@
       <c r="B121" s="0" t="s">
         <v>265</v>
       </c>
-      <c r="C121" s="4" t="n">
+      <c r="C121" s="5" t="n">
         <v>1985</v>
       </c>
       <c r="D121" s="3"/>
@@ -3040,7 +3043,7 @@
       <c r="B122" s="0" t="s">
         <v>269</v>
       </c>
-      <c r="C122" s="4" t="n">
+      <c r="C122" s="5" t="n">
         <v>1995</v>
       </c>
       <c r="D122" s="3"/>
@@ -3061,7 +3064,7 @@
       <c r="B123" s="0" t="s">
         <v>273</v>
       </c>
-      <c r="C123" s="4" t="n">
+      <c r="C123" s="5" t="n">
         <v>2005</v>
       </c>
       <c r="D123" s="3"/>
@@ -3082,7 +3085,7 @@
       <c r="B124" s="0" t="s">
         <v>277</v>
       </c>
-      <c r="C124" s="4" t="n">
+      <c r="C124" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="D124" s="3"/>
@@ -3094,7 +3097,7 @@
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C125" s="4"/>
+      <c r="C125" s="5"/>
       <c r="D125" s="3"/>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3104,7 +3107,7 @@
       <c r="B126" s="0" t="s">
         <v>281</v>
       </c>
-      <c r="C126" s="4" t="n">
+      <c r="C126" s="5" t="n">
         <v>1965</v>
       </c>
       <c r="D126" s="3" t="s">
@@ -3124,7 +3127,7 @@
       <c r="B127" s="0" t="s">
         <v>286</v>
       </c>
-      <c r="C127" s="4" t="n">
+      <c r="C127" s="5" t="n">
         <v>1985</v>
       </c>
       <c r="D127" s="3"/>
@@ -3142,7 +3145,7 @@
       <c r="B128" s="0" t="s">
         <v>290</v>
       </c>
-      <c r="C128" s="4" t="n">
+      <c r="C128" s="5" t="n">
         <v>2005</v>
       </c>
       <c r="D128" s="3"/>
@@ -3163,7 +3166,7 @@
       <c r="B129" s="0" t="s">
         <v>295</v>
       </c>
-      <c r="C129" s="4" t="n">
+      <c r="C129" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="D129" s="3"/>
@@ -3175,7 +3178,7 @@
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C130" s="4"/>
+      <c r="C130" s="5"/>
       <c r="D130" s="3"/>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3185,7 +3188,7 @@
       <c r="B131" s="0" t="s">
         <v>299</v>
       </c>
-      <c r="C131" s="4" t="n">
+      <c r="C131" s="5" t="n">
         <v>1965</v>
       </c>
       <c r="D131" s="3" t="s">
@@ -3205,7 +3208,7 @@
       <c r="B132" s="0" t="s">
         <v>304</v>
       </c>
-      <c r="C132" s="4" t="n">
+      <c r="C132" s="5" t="n">
         <v>1975</v>
       </c>
       <c r="D132" s="3"/>
@@ -3223,7 +3226,7 @@
       <c r="B133" s="0" t="s">
         <v>308</v>
       </c>
-      <c r="C133" s="4" t="n">
+      <c r="C133" s="5" t="n">
         <v>1985</v>
       </c>
       <c r="D133" s="3"/>
@@ -3244,7 +3247,7 @@
       <c r="B134" s="0" t="s">
         <v>313</v>
       </c>
-      <c r="C134" s="4" t="n">
+      <c r="C134" s="5" t="n">
         <v>1995</v>
       </c>
       <c r="D134" s="3"/>
@@ -3265,7 +3268,7 @@
       <c r="B135" s="0" t="s">
         <v>318</v>
       </c>
-      <c r="C135" s="4" t="n">
+      <c r="C135" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="D135" s="3" t="s">
@@ -3279,7 +3282,7 @@
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C136" s="4"/>
+      <c r="C136" s="5"/>
       <c r="D136" s="3"/>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3289,7 +3292,7 @@
       <c r="B137" s="0" t="s">
         <v>323</v>
       </c>
-      <c r="C137" s="4" t="n">
+      <c r="C137" s="5" t="n">
         <v>1965</v>
       </c>
       <c r="D137" s="3" t="s">
@@ -3309,7 +3312,7 @@
       <c r="B138" s="0" t="s">
         <v>328</v>
       </c>
-      <c r="C138" s="4" t="n">
+      <c r="C138" s="5" t="n">
         <v>1975</v>
       </c>
       <c r="D138" s="3" t="s">
@@ -3329,7 +3332,7 @@
       <c r="B139" s="0" t="s">
         <v>332</v>
       </c>
-      <c r="C139" s="4" t="n">
+      <c r="C139" s="5" t="n">
         <v>1985</v>
       </c>
       <c r="D139" s="3" t="s">
@@ -3343,7 +3346,7 @@
       <c r="B140" s="0" t="s">
         <v>334</v>
       </c>
-      <c r="C140" s="4" t="n">
+      <c r="C140" s="5" t="n">
         <v>1995</v>
       </c>
       <c r="D140" s="3" t="s">
@@ -3360,7 +3363,7 @@
       <c r="B141" s="0" t="s">
         <v>337</v>
       </c>
-      <c r="C141" s="4" t="n">
+      <c r="C141" s="5" t="n">
         <v>2015</v>
       </c>
       <c r="D141" s="3" t="s">
@@ -3371,42 +3374,42 @@
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C142" s="4"/>
+      <c r="C142" s="5"/>
       <c r="D142" s="3"/>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C143" s="4"/>
+      <c r="C143" s="5"/>
       <c r="D143" s="3"/>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="C144" s="4"/>
+      <c r="C144" s="5"/>
       <c r="D144" s="3"/>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B145" s="0" t="s">
         <v>340</v>
       </c>
-      <c r="C145" s="4"/>
+      <c r="C145" s="5"/>
       <c r="D145" s="3" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C146" s="4"/>
+      <c r="C146" s="5"/>
       <c r="D146" s="3"/>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
         <v>342</v>
       </c>
-      <c r="C147" s="4"/>
+      <c r="C147" s="5"/>
       <c r="D147" s="3"/>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C148" s="4"/>
+      <c r="C148" s="5"/>
       <c r="D148" s="3"/>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3416,7 +3419,7 @@
       <c r="B149" s="0" t="s">
         <v>344</v>
       </c>
-      <c r="C149" s="4" t="s">
+      <c r="C149" s="5" t="s">
         <v>345</v>
       </c>
       <c r="D149" s="3" t="s">
@@ -3439,7 +3442,7 @@
       <c r="B150" s="0" t="s">
         <v>351</v>
       </c>
-      <c r="C150" s="4" t="s">
+      <c r="C150" s="5" t="s">
         <v>352</v>
       </c>
       <c r="D150" s="3"/>
@@ -3460,7 +3463,7 @@
       <c r="B151" s="0" t="s">
         <v>357</v>
       </c>
-      <c r="C151" s="4" t="s">
+      <c r="C151" s="5" t="s">
         <v>358</v>
       </c>
       <c r="D151" s="3"/>
@@ -3481,7 +3484,7 @@
       <c r="B152" s="0" t="s">
         <v>363</v>
       </c>
-      <c r="C152" s="4" t="s">
+      <c r="C152" s="5" t="s">
         <v>364</v>
       </c>
       <c r="D152" s="3"/>
@@ -3490,20 +3493,20 @@
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C153" s="4"/>
+      <c r="C153" s="5"/>
       <c r="D153" s="3"/>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B154" s="0" t="s">
         <v>366</v>
       </c>
-      <c r="C154" s="4"/>
+      <c r="C154" s="5"/>
       <c r="D154" s="3" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C155" s="4"/>
+      <c r="C155" s="5"/>
       <c r="D155" s="3"/>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3513,7 +3516,7 @@
       <c r="B156" s="0" t="s">
         <v>369</v>
       </c>
-      <c r="C156" s="4" t="s">
+      <c r="C156" s="5" t="s">
         <v>345</v>
       </c>
       <c r="D156" s="3" t="s">
@@ -3533,7 +3536,7 @@
       <c r="B157" s="0" t="s">
         <v>374</v>
       </c>
-      <c r="C157" s="4" t="s">
+      <c r="C157" s="5" t="s">
         <v>352</v>
       </c>
       <c r="D157" s="3" t="s">
@@ -3550,7 +3553,7 @@
       <c r="B158" s="0" t="s">
         <v>377</v>
       </c>
-      <c r="C158" s="4" t="s">
+      <c r="C158" s="5" t="s">
         <v>358</v>
       </c>
       <c r="D158" s="3" t="s">
@@ -3570,7 +3573,7 @@
       <c r="B159" s="0" t="s">
         <v>381</v>
       </c>
-      <c r="C159" s="4" t="s">
+      <c r="C159" s="5" t="s">
         <v>364</v>
       </c>
       <c r="D159" s="3" t="s">
@@ -3581,7 +3584,7 @@
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C160" s="4"/>
+      <c r="C160" s="5"/>
       <c r="D160" s="3"/>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3591,7 +3594,7 @@
       <c r="B161" s="0" t="s">
         <v>384</v>
       </c>
-      <c r="C161" s="4" t="s">
+      <c r="C161" s="5" t="s">
         <v>345</v>
       </c>
       <c r="D161" s="0" t="s">
@@ -3608,7 +3611,7 @@
       <c r="B162" s="0" t="s">
         <v>388</v>
       </c>
-      <c r="C162" s="4" t="s">
+      <c r="C162" s="5" t="s">
         <v>352</v>
       </c>
       <c r="D162" s="0" t="s">
@@ -3628,7 +3631,7 @@
       <c r="B163" s="0" t="s">
         <v>393</v>
       </c>
-      <c r="C163" s="4" t="s">
+      <c r="C163" s="5" t="s">
         <v>352</v>
       </c>
       <c r="D163" s="3" t="s">
@@ -3651,7 +3654,7 @@
       <c r="B164" s="0" t="s">
         <v>399</v>
       </c>
-      <c r="C164" s="4" t="s">
+      <c r="C164" s="5" t="s">
         <v>358</v>
       </c>
       <c r="D164" s="3"/>
@@ -3669,7 +3672,7 @@
       <c r="B165" s="0" t="s">
         <v>403</v>
       </c>
-      <c r="C165" s="4" t="s">
+      <c r="C165" s="5" t="s">
         <v>364</v>
       </c>
       <c r="D165" s="3"/>
@@ -3681,20 +3684,20 @@
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C166" s="4"/>
+      <c r="C166" s="5"/>
       <c r="D166" s="3"/>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B167" s="0" t="s">
         <v>406</v>
       </c>
-      <c r="C167" s="4"/>
+      <c r="C167" s="5"/>
       <c r="D167" s="3" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C168" s="4"/>
+      <c r="C168" s="5"/>
       <c r="D168" s="3"/>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3704,7 +3707,7 @@
       <c r="B169" s="0" t="s">
         <v>409</v>
       </c>
-      <c r="C169" s="4" t="s">
+      <c r="C169" s="5" t="s">
         <v>345</v>
       </c>
       <c r="D169" s="3"/>
@@ -3725,7 +3728,7 @@
       <c r="B170" s="0" t="s">
         <v>414</v>
       </c>
-      <c r="C170" s="4" t="s">
+      <c r="C170" s="5" t="s">
         <v>352</v>
       </c>
       <c r="D170" s="3"/>
@@ -3746,7 +3749,7 @@
       <c r="B171" s="0" t="s">
         <v>419</v>
       </c>
-      <c r="C171" s="4" t="s">
+      <c r="C171" s="5" t="s">
         <v>358</v>
       </c>
       <c r="D171" s="3"/>
@@ -3767,105 +3770,135 @@
       <c r="B172" s="0" t="s">
         <v>424</v>
       </c>
-      <c r="C172" s="4" t="s">
+      <c r="C172" s="5" t="s">
         <v>364</v>
       </c>
       <c r="D172" s="3"/>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C173" s="4"/>
+      <c r="C173" s="5"/>
       <c r="D173" s="3"/>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B174" s="0" t="s">
         <v>425</v>
       </c>
-      <c r="C174" s="4"/>
+      <c r="C174" s="5"/>
       <c r="D174" s="3" t="s">
         <v>426</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C175" s="4"/>
+      <c r="C175" s="5"/>
       <c r="D175" s="3"/>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="1" t="s">
         <v>427</v>
       </c>
-      <c r="C176" s="4"/>
+      <c r="C176" s="5"/>
       <c r="D176" s="3"/>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C178" s="4"/>
+      <c r="C178" s="5"/>
       <c r="D178" s="3"/>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="s">
         <v>428</v>
       </c>
-      <c r="C179" s="4"/>
+      <c r="B179" s="0" t="s">
+        <v>429</v>
+      </c>
+      <c r="C179" s="5" t="n">
+        <v>1975</v>
+      </c>
       <c r="D179" s="3"/>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="s">
-        <v>429</v>
-      </c>
-      <c r="C180" s="4"/>
+        <v>430</v>
+      </c>
+      <c r="B180" s="0" t="s">
+        <v>431</v>
+      </c>
+      <c r="C180" s="5" t="n">
+        <v>1995</v>
+      </c>
       <c r="D180" s="3"/>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C181" s="4"/>
+      <c r="A181" s="0" t="s">
+        <v>432</v>
+      </c>
+      <c r="B181" s="0" t="s">
+        <v>433</v>
+      </c>
+      <c r="C181" s="5" t="n">
+        <v>2015</v>
+      </c>
       <c r="D181" s="3"/>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="0" t="s">
-        <v>430</v>
-      </c>
-      <c r="C182" s="4" t="n">
-        <v>1965</v>
-      </c>
-      <c r="D182" s="3" t="s">
-        <v>431</v>
-      </c>
+      <c r="C182" s="5"/>
+      <c r="D182" s="3"/>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="0" t="s">
-        <v>432</v>
-      </c>
-      <c r="C183" s="4" t="n">
-        <v>1965</v>
-      </c>
-      <c r="D183" s="3" t="s">
-        <v>433</v>
-      </c>
+      <c r="C183" s="5"/>
+      <c r="D183" s="3"/>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="0" t="s">
-        <v>434</v>
-      </c>
-      <c r="C184" s="4" t="n">
-        <v>1985</v>
-      </c>
+      <c r="C184" s="5"/>
       <c r="D184" s="3"/>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="s">
+        <v>434</v>
+      </c>
+      <c r="C185" s="5" t="n">
+        <v>1965</v>
+      </c>
+      <c r="D185" s="3" t="s">
         <v>435</v>
       </c>
-      <c r="C185" s="4" t="n">
-        <v>2005</v>
-      </c>
-      <c r="D185" s="3"/>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="s">
         <v>436</v>
       </c>
-      <c r="C186" s="4" t="n">
+      <c r="C186" s="5" t="n">
+        <v>1965</v>
+      </c>
+      <c r="D186" s="3" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="0" t="s">
+        <v>438</v>
+      </c>
+      <c r="C187" s="5" t="n">
+        <v>1985</v>
+      </c>
+      <c r="D187" s="3"/>
+    </row>
+    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="0" t="s">
+        <v>439</v>
+      </c>
+      <c r="C188" s="5" t="n">
+        <v>2005</v>
+      </c>
+      <c r="D188" s="3"/>
+    </row>
+    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="0" t="s">
+        <v>440</v>
+      </c>
+      <c r="C189" s="5" t="n">
         <v>2015</v>
       </c>
-      <c r="D186" s="3"/>
+      <c r="D189" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>